<commit_message>
add gitignore file and modify the database file
</commit_message>
<xml_diff>
--- a/document/数据库设计/危废电子联单系统数据库设计.xlsx
+++ b/document/数据库设计/危废电子联单系统数据库设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" tabRatio="785" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" tabRatio="785" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="用户（user)" sheetId="18" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="444">
   <si>
     <t>序号</t>
   </si>
@@ -1370,19 +1370,55 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>waste_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主要危险成分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waste_ingredient</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>否</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>waste_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主要危险成分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>waste_ingredient</t>
+    <t>序号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字段名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库字段名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据长度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许空值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>device_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1390,35 +1426,239 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字段名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据库字段名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据长度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>允许空值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设备编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>device_id</t>
+    <t>设备名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>device_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>device_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备序列号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>device_serial_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备归属企业编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ownership_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备运行状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>device_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tinyint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0表示运行正常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:admin/1:country/2:province/3:city/4:district/5:production/6:transport/7:reception</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车辆1编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vehicle_id_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车辆2编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vehicle_id_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waste_weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waste_package</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waste_transport_goal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emergency_measure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waste_shipper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waste_destination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waste_transport_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrier_1_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrier_1_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_date_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_license_num_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_pass_by_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_destination_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrier_2_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrier_2_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_date_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_license_num_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_start_point_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_pass_by_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_destination_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiving_unit_license_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiver_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiver_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receive_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waste_disposal_method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiving_unit_principal_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiving_unit_audit_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键，vehicle表的主键</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备归属企业类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ownership_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tinyint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5:production/6:transport/7:reception</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_start_point_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>production_unit_legal_person_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transport_unit_legal_person_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>receiving_unit_legal_person_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>production_unit_legal_person_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键fk_user_id_production，user表的主键user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键fk_user_id_transport，user表的主键user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键fk_user_id_receiving，user表的主键user_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1426,15 +1666,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联单ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>manifest_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>否</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>设备名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>device_name</t>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键fk_waste_id，waste表的主键waste_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键fk_production_unit_id，production_unit表的主键production_unit_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键fk_transport_unit_id，transport_unit表的主键transport_unit_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键fk_receiving_unit_id，receiving_unit表的主键receiving_unit_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键，自动递增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>产生单位主要危废物</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>production_unit_waste</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1442,243 +1726,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>设备类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>device_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设备序列号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>device_serial_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设备归属企业编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ownership_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设备运行状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>device_status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tinyint</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0表示运行正常</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0:admin/1:country/2:province/3:city/4:district/5:production/6:transport/7:reception</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>车辆1编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vehicle_id_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>车辆2编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vehicle_id_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>waste_weight</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>waste_package</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>waste_transport_goal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>emergency_measure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>waste_shipper</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>waste_destination</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>waste_transport_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>carrier_1_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>carrier_1_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_date_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_license_num_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_pass_by_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_destination_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>carrier_2_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>carrier_2_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_date_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_license_num_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_start_point_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_pass_by_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_destination_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>receiving_unit_license_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>receiver_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>receiver_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>receive_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>waste_disposal_method</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>receiving_unit_principal_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>receiving_unit_audit_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>外键，vehicle表的主键</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设备归属企业类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ownership_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tinyint</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5:production/6:transport/7:reception</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_start_point_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>production_unit_legal_person_code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>transport_unit_legal_person_code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>receiving_unit_legal_person_code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>production_unit_legal_person_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>外键fk_user_id_production，user表的主键user_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>外键fk_user_id_transport，user表的主键user_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>外键fk_user_id_receiving，user表的主键user_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>联单ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>manifest_id</t>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>例子：4，waste_id,waste_id,waste_id,waste_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类别编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waste_category</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1686,55 +1746,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>外键fk_waste_id，waste表的主键waste_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>外键fk_production_unit_id，production_unit表的主键production_unit_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>外键fk_transport_unit_id，transport_unit表的主键transport_unit_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>外键fk_receiving_unit_id，receiving_unit表的主键receiving_unit_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主键，自动递增</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>产生单位主要危废物</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>production_unit_waste</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>是</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>例子：4，waste_id,waste_id,waste_id,waste_id</t>
+    <t>waste_category_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>废物类别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>行业来源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waste_from</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2326,10 +2354,10 @@
         <v>11</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -2349,10 +2377,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -2372,7 +2400,7 @@
         <v>255</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -2392,7 +2420,7 @@
         <v>255</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -2452,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
@@ -2472,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
@@ -2492,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -2512,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -2532,7 +2560,7 @@
         <v>255</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -2552,7 +2580,7 @@
         <v>255</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
@@ -2572,7 +2600,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
@@ -2592,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -2606,7 +2634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -2659,7 +2687,7 @@
         <v>109</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -2682,7 +2710,7 @@
         <v>245</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -3029,7 +3057,7 @@
         <v>122</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>188</v>
@@ -3050,7 +3078,7 @@
         <v>123</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>188</v>
@@ -3169,22 +3197,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="32" t="s">
+        <v>431</v>
+      </c>
+      <c r="C27" s="32" t="s">
         <v>432</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="D27" s="32" t="s">
         <v>433</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="E27" s="32">
+        <v>255</v>
+      </c>
+      <c r="F27" s="33" t="s">
         <v>434</v>
       </c>
-      <c r="E27" s="32">
-        <v>255</v>
-      </c>
-      <c r="F27" s="33" t="s">
+      <c r="G27" s="32" t="s">
         <v>435</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -3250,7 +3278,7 @@
         <v>186</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -3273,7 +3301,7 @@
         <v>186</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -3623,7 +3651,7 @@
         <v>288</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E20" s="18">
         <v>0</v>
@@ -3644,7 +3672,7 @@
         <v>289</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E21" s="18">
         <v>0</v>
@@ -3704,7 +3732,7 @@
         <v>141</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>190</v>
@@ -3902,7 +3930,7 @@
         <v>186</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -3925,7 +3953,7 @@
         <v>186</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -4275,7 +4303,7 @@
         <v>317</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E20" s="18">
         <v>0</v>
@@ -4296,7 +4324,7 @@
         <v>318</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E21" s="18">
         <v>0</v>
@@ -4356,7 +4384,7 @@
         <v>173</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>190</v>
@@ -5656,22 +5684,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>422</v>
-      </c>
       <c r="D2" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E2" s="10">
         <v>11</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.15">
@@ -5685,7 +5713,7 @@
         <v>328</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E3" s="2">
         <v>255</v>
@@ -5705,7 +5733,7 @@
         <v>329</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E4" s="4">
         <v>11</v>
@@ -5714,7 +5742,7 @@
         <v>79</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.15">
@@ -5728,7 +5756,7 @@
         <v>270</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E5" s="4">
         <v>11</v>
@@ -5737,7 +5765,7 @@
         <v>79</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.15">
@@ -5751,7 +5779,7 @@
         <v>332</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E6" s="4">
         <v>11</v>
@@ -5760,7 +5788,7 @@
         <v>79</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.15">
@@ -5771,10 +5799,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E7" s="4">
         <v>11</v>
@@ -5783,7 +5811,7 @@
         <v>79</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.15">
@@ -5794,7 +5822,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>7</v>
@@ -5814,7 +5842,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
@@ -5834,7 +5862,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>7</v>
@@ -5854,7 +5882,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>7</v>
@@ -5878,7 +5906,7 @@
         <v>26</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>7</v>
@@ -5902,7 +5930,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>7</v>
@@ -5926,7 +5954,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>46</v>
@@ -5948,7 +5976,7 @@
         <v>68</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>96</v>
@@ -5968,7 +5996,7 @@
         <v>69</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>96</v>
@@ -5988,7 +6016,7 @@
         <v>54</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>97</v>
@@ -6003,10 +6031,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>375</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>96</v>
@@ -6018,7 +6046,7 @@
         <v>98</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.15">
@@ -6029,7 +6057,7 @@
         <v>70</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>96</v>
@@ -6049,7 +6077,7 @@
         <v>56</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>96</v>
@@ -6069,7 +6097,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>96</v>
@@ -6089,7 +6117,7 @@
         <v>58</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>96</v>
@@ -6109,7 +6137,7 @@
         <v>71</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>96</v>
@@ -6129,7 +6157,7 @@
         <v>72</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>96</v>
@@ -6149,7 +6177,7 @@
         <v>54</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>97</v>
@@ -6164,10 +6192,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>376</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>377</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>96</v>
@@ -6179,7 +6207,7 @@
         <v>98</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.15">
@@ -6190,7 +6218,7 @@
         <v>70</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>96</v>
@@ -6210,7 +6238,7 @@
         <v>56</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>96</v>
@@ -6230,7 +6258,7 @@
         <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>96</v>
@@ -6250,7 +6278,7 @@
         <v>58</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>96</v>
@@ -6270,7 +6298,7 @@
         <v>73</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>96</v>
@@ -6290,7 +6318,7 @@
         <v>74</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>96</v>
@@ -6310,7 +6338,7 @@
         <v>60</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>96</v>
@@ -6330,7 +6358,7 @@
         <v>59</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>108</v>
@@ -6348,7 +6376,7 @@
         <v>75</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>96</v>
@@ -6368,7 +6396,7 @@
         <v>76</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>96</v>
@@ -6388,7 +6416,7 @@
         <v>77</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>108</v>
@@ -6407,10 +6435,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6462,7 +6490,7 @@
         <v>109</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -6482,7 +6510,7 @@
         <v>255</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="G3" s="18"/>
     </row>
@@ -6491,10 +6519,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>347</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>348</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>235</v>
@@ -6503,7 +6531,7 @@
         <v>255</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>345</v>
+        <v>98</v>
       </c>
       <c r="G4" s="18"/>
     </row>
@@ -6524,7 +6552,7 @@
         <v>255</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>345</v>
+        <v>98</v>
       </c>
       <c r="G5" s="18"/>
     </row>
@@ -6545,7 +6573,7 @@
         <v>255</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>345</v>
+        <v>98</v>
       </c>
       <c r="G6" s="18"/>
     </row>
@@ -6566,9 +6594,77 @@
         <v>255</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>345</v>
+        <v>98</v>
       </c>
       <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="32">
+        <v>7</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>436</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>440</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>438</v>
+      </c>
+      <c r="E8" s="32">
+        <v>255</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="32">
+        <v>8</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>441</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>437</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>438</v>
+      </c>
+      <c r="E9" s="32">
+        <v>255</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="32">
+        <v>9</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>442</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>443</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>438</v>
+      </c>
+      <c r="E10" s="32">
+        <v>255</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6594,22 +6690,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>354</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>355</v>
       </c>
       <c r="G1" s="22"/>
     </row>
@@ -6618,22 +6714,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="D2" s="18" t="s">
         <v>357</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>358</v>
       </c>
       <c r="E2" s="18">
         <v>11</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -6641,19 +6737,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>362</v>
-      </c>
       <c r="E3" s="18">
         <v>255</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G3" s="22"/>
     </row>
@@ -6662,19 +6758,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>363</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>364</v>
-      </c>
       <c r="D4" s="18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E4" s="18">
         <v>255</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G4" s="22"/>
     </row>
@@ -6683,19 +6779,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>366</v>
-      </c>
       <c r="D5" s="18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E5" s="18">
         <v>255</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G5" s="22"/>
     </row>
@@ -6704,22 +6800,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>406</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>407</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>408</v>
       </c>
       <c r="E6" s="18">
         <v>4</v>
       </c>
       <c r="F6" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="G6" s="30" t="s">
         <v>409</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -6727,19 +6823,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>367</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>368</v>
-      </c>
       <c r="D7" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E7" s="18">
         <v>11</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G7" s="22"/>
     </row>
@@ -6748,22 +6844,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>369</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="D8" s="18" t="s">
         <v>370</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>371</v>
       </c>
       <c r="E8" s="18">
         <v>4</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify the database xlsx
</commit_message>
<xml_diff>
--- a/document/数据库设计/危废电子联单系统数据库设计.xlsx
+++ b/document/数据库设计/危废电子联单系统数据库设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" tabRatio="785" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" tabRatio="785" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="用户（user)" sheetId="18" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="449">
   <si>
     <t>序号</t>
   </si>
@@ -1763,6 +1763,217 @@
   </si>
   <si>
     <t>waste_from</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联单状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>manifest_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tinyint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>：产生单位备案；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>：运输单位审核；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>：运输单位退回；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>：环保局审核通过；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>：环保局退回；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>：产生单位登记联单；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>：处置单位接受联单；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>：处置单位退回联单。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>：若</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>退回则环保局审核；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>：审核通过后企业能够修改，重新提交。</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1906,7 +2117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1992,6 +2203,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5640,10 +5860,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5652,7 +5872,7 @@
     <col min="2" max="2" width="23.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="111.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
     <col min="9" max="9" width="9.125" style="1" customWidth="1"/>
     <col min="10" max="10" width="31.75" style="1" bestFit="1" customWidth="1"/>
@@ -6330,7 +6550,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -6350,7 +6570,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -6368,7 +6588,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -6388,7 +6608,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -6408,7 +6628,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -6424,6 +6644,29 @@
       <c r="E37" s="9"/>
       <c r="F37" s="13" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A38" s="34">
+        <v>37</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>444</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>445</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="E38" s="34">
+        <v>4</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>447</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -6437,7 +6680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD10"/>
     </sheetView>
   </sheetViews>

</xml_diff>